<commit_message>
Fixed ordering in the tree view
</commit_message>
<xml_diff>
--- a/tests/_data/Ordering.xlsx
+++ b/tests/_data/Ordering.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167">
   <si>
     <t>identifier</t>
   </si>
@@ -73,9 +73,6 @@
   </si>
   <si>
     <t>2017-09-27 17:00:40</t>
-  </si>
-  <si>
-    <t>Private Draft</t>
   </si>
   <si>
     <t>fullStatement</t>
@@ -527,10 +524,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -563,8 +560,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -579,16 +584,17 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -607,9 +613,38 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -624,46 +659,8 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -676,16 +673,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -706,25 +703,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -736,25 +763,73 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -766,19 +841,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -790,37 +865,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -832,55 +877,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -918,6 +915,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -933,20 +939,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -977,17 +980,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -996,142 +993,142 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
@@ -1466,7 +1463,7 @@
   <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="12.75" outlineLevelRow="1"/>
@@ -1537,9 +1534,7 @@
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
-      <c r="K2" s="1" t="s">
-        <v>19</v>
-      </c>
+      <c r="K2" s="1"/>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
@@ -1557,7 +1552,7 @@
   <dimension ref="A1:N29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="12.75"/>
@@ -1570,22 +1565,22 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>25</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>14</v>
@@ -1594,55 +1589,55 @@
         <v>8</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>27</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>13</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="N1" s="1"/>
     </row>
     <row r="2" s="1" customFormat="1" spans="1:13">
       <c r="A2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:14">
       <c r="A3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>38</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
@@ -1651,26 +1646,26 @@
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N3" s="1"/>
     </row>
     <row r="4" spans="1:14">
       <c r="A4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
@@ -1679,26 +1674,26 @@
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
       <c r="M4" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N4" s="1"/>
     </row>
     <row r="5" spans="1:14">
       <c r="A5" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>48</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
@@ -1707,22 +1702,22 @@
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
       <c r="M5" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N5" s="1"/>
     </row>
     <row r="6" spans="1:14">
       <c r="A6" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>53</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
@@ -1733,22 +1728,22 @@
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
       <c r="M6" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N6" s="1"/>
     </row>
     <row r="7" spans="1:14">
       <c r="A7" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>57</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
@@ -1759,78 +1754,78 @@
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
       <c r="M7" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N7" s="1"/>
     </row>
     <row r="8" spans="1:14">
       <c r="A8" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="C8" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="D8" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>61</v>
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
       <c r="M8" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N8" s="1"/>
     </row>
     <row r="9" spans="1:14">
       <c r="A9" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="C9" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="D9" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>66</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
       <c r="M9" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N9" s="1"/>
     </row>
     <row r="10" spans="1:14">
       <c r="A10" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="C10" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>70</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>71</v>
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
@@ -1841,22 +1836,22 @@
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
       <c r="M10" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N10" s="1"/>
     </row>
     <row r="11" spans="1:14">
       <c r="A11" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="C11" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="D11" s="1" t="s">
         <v>74</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>75</v>
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
@@ -1867,22 +1862,22 @@
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
       <c r="M11" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N11" s="1"/>
     </row>
     <row r="12" spans="1:14">
       <c r="A12" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="C12" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="D12" s="1" t="s">
         <v>78</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>79</v>
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
@@ -1893,78 +1888,78 @@
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
       <c r="M12" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N12" s="1"/>
     </row>
     <row r="13" spans="1:14">
       <c r="A13" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="C13" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="D13" s="1" t="s">
         <v>82</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>83</v>
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
       <c r="M13" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N13" s="1"/>
     </row>
     <row r="14" spans="1:14">
       <c r="A14" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="C14" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="D14" s="1" t="s">
         <v>87</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>88</v>
       </c>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
       <c r="M14" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N14" s="1"/>
     </row>
     <row r="15" spans="1:14">
       <c r="A15" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="C15" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="D15" s="1" t="s">
         <v>92</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>93</v>
       </c>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
@@ -1975,22 +1970,22 @@
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
       <c r="M15" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N15" s="1"/>
     </row>
     <row r="16" spans="1:14">
       <c r="A16" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="C16" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="D16" s="1" t="s">
         <v>96</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>97</v>
       </c>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
@@ -2001,78 +1996,78 @@
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
       <c r="M16" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N16" s="1"/>
     </row>
     <row r="17" spans="1:14">
       <c r="A17" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="C17" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="D17" s="1" t="s">
         <v>100</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>101</v>
       </c>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
       <c r="H17" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
       <c r="M17" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N17" s="1"/>
     </row>
     <row r="18" spans="1:14">
       <c r="A18" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="C18" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="D18" s="1" t="s">
         <v>105</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>106</v>
       </c>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
       <c r="H18" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
       <c r="M18" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N18" s="1"/>
     </row>
     <row r="19" spans="1:14">
       <c r="A19" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="C19" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="D19" s="1" t="s">
         <v>110</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>111</v>
       </c>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
@@ -2083,78 +2078,78 @@
       <c r="K19" s="1"/>
       <c r="L19" s="1"/>
       <c r="M19" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N19" s="1"/>
     </row>
     <row r="20" spans="1:14">
       <c r="A20" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="C20" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="D20" s="1" t="s">
         <v>114</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>115</v>
       </c>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
       <c r="H20" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
       <c r="M20" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N20" s="1"/>
     </row>
     <row r="21" spans="1:14">
       <c r="A21" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="C21" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="D21" s="1" t="s">
         <v>119</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>120</v>
       </c>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
       <c r="H21" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
       <c r="M21" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N21" s="1"/>
     </row>
     <row r="22" spans="1:14">
       <c r="A22" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="C22" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="D22" s="1" t="s">
         <v>124</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>125</v>
       </c>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
@@ -2165,22 +2160,22 @@
       <c r="K22" s="1"/>
       <c r="L22" s="1"/>
       <c r="M22" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N22" s="1"/>
     </row>
     <row r="23" spans="1:14">
       <c r="A23" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="C23" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="D23" s="1" t="s">
         <v>128</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>129</v>
       </c>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
@@ -2191,50 +2186,50 @@
       <c r="K23" s="1"/>
       <c r="L23" s="1"/>
       <c r="M23" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N23" s="1"/>
     </row>
     <row r="24" spans="1:14">
       <c r="A24" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="C24" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="D24" s="1" t="s">
         <v>132</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>133</v>
       </c>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
       <c r="H24" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
       <c r="L24" s="1"/>
       <c r="M24" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N24" s="1"/>
     </row>
     <row r="25" spans="1:14">
       <c r="A25" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B25" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="C25" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="D25" s="1" t="s">
         <v>137</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>138</v>
       </c>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
@@ -2245,50 +2240,50 @@
       <c r="K25" s="1"/>
       <c r="L25" s="1"/>
       <c r="M25" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N25" s="1"/>
     </row>
     <row r="26" spans="1:14">
       <c r="A26" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="C26" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="D26" s="1" t="s">
         <v>141</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>142</v>
       </c>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
       <c r="H26" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="I26" s="1"/>
       <c r="J26" s="1"/>
       <c r="K26" s="1"/>
       <c r="L26" s="1"/>
       <c r="M26" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="N26" s="1"/>
     </row>
     <row r="27" spans="1:14">
       <c r="A27" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="C27" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="D27" s="1" t="s">
         <v>147</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>148</v>
       </c>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
@@ -2299,50 +2294,50 @@
       <c r="K27" s="1"/>
       <c r="L27" s="1"/>
       <c r="M27" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="N27" s="1"/>
     </row>
     <row r="28" spans="1:14">
       <c r="A28" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="C28" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="D28" s="1" t="s">
         <v>152</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>153</v>
       </c>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
       <c r="H28" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
       <c r="K28" s="1"/>
       <c r="L28" s="1"/>
       <c r="M28" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="N28" s="1"/>
     </row>
     <row r="29" spans="1:14">
       <c r="A29" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B29" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="C29" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="D29" s="1" t="s">
         <v>158</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>159</v>
       </c>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
@@ -2353,7 +2348,7 @@
       <c r="K29" s="1"/>
       <c r="L29" s="1"/>
       <c r="M29" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="N29" s="1"/>
     </row>
@@ -2379,31 +2374,31 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>167</v>
-      </c>
       <c r="J1" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K1" s="1"/>
     </row>

</xml_diff>